<commit_message>
unit test fixes & regression errors they uncovered: - remove 'telescope' buckets - updated cookbook tests - handling of the test database changed in django
</commit_message>
<xml_diff>
--- a/doc/cookbook/resource/resource-skills.xlsx
+++ b/doc/cookbook/resource/resource-skills.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="323" yWindow="585" windowWidth="20798" windowHeight="5243" tabRatio="665" activeTab="15"/>
+    <workbookView xWindow="323" yWindow="585" windowWidth="20798" windowHeight="5243" tabRatio="763" firstSheet="1" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="buffer" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="305">
   <si>
     <t>name</t>
   </si>
@@ -946,6 +946,9 @@
   </si>
   <si>
     <t>MINCOSTPENALTY</t>
+  </si>
+  <si>
+    <t>level</t>
   </si>
 </sst>
 </file>
@@ -3587,60 +3590,81 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="18.9296875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C1" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>96</v>
       </c>
       <c r="B2" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>88</v>
       </c>
       <c r="B3" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>85</v>
       </c>
       <c r="B4" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>92</v>
       </c>
       <c r="B5" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>81</v>
       </c>
       <c r="B6" t="s">
         <v>287</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3652,7 +3676,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
tests cookbook: models updated
</commit_message>
<xml_diff>
--- a/doc/cookbook/resource/resource-skills.xlsx
+++ b/doc/cookbook/resource/resource-skills.xlsx
@@ -5,36 +5,37 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\develop\frepple.community\doc\cookbook\resource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frePPLe\Documents\frePPLe_comunity\doc\cookbook\resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="323" yWindow="585" windowWidth="20798" windowHeight="5243" tabRatio="763" activeTab="4"/>
+    <workbookView xWindow="323" yWindow="585" windowWidth="20798" windowHeight="5243" tabRatio="852" activeTab="8"/>
   </bookViews>
   <sheets>
-    <sheet name="buffer" sheetId="1" r:id="rId1"/>
-    <sheet name="calendar bucket" sheetId="2" r:id="rId2"/>
-    <sheet name="calendar" sheetId="3" r:id="rId3"/>
-    <sheet name="customer" sheetId="4" r:id="rId4"/>
-    <sheet name="demand" sheetId="5" r:id="rId5"/>
-    <sheet name="flow" sheetId="6" r:id="rId6"/>
-    <sheet name="item" sheetId="7" r:id="rId7"/>
-    <sheet name="load" sheetId="8" r:id="rId8"/>
-    <sheet name="location" sheetId="9" r:id="rId9"/>
-    <sheet name="operation" sheetId="11" r:id="rId10"/>
-    <sheet name="resource skill" sheetId="12" r:id="rId11"/>
-    <sheet name="resource" sheetId="13" r:id="rId12"/>
-    <sheet name="skill" sheetId="15" r:id="rId13"/>
-    <sheet name="bucket date" sheetId="17" r:id="rId14"/>
-    <sheet name="bucket" sheetId="18" r:id="rId15"/>
-    <sheet name="parameter" sheetId="19" r:id="rId16"/>
+    <sheet name="itemoperation" sheetId="20" r:id="rId1"/>
+    <sheet name="buffer" sheetId="1" r:id="rId2"/>
+    <sheet name="calendar bucket" sheetId="2" r:id="rId3"/>
+    <sheet name="calendar" sheetId="3" r:id="rId4"/>
+    <sheet name="customer" sheetId="4" r:id="rId5"/>
+    <sheet name="demand" sheetId="5" r:id="rId6"/>
+    <sheet name="operationmaterial" sheetId="6" r:id="rId7"/>
+    <sheet name="item" sheetId="7" r:id="rId8"/>
+    <sheet name="operationresource" sheetId="8" r:id="rId9"/>
+    <sheet name="location" sheetId="9" r:id="rId10"/>
+    <sheet name="operation" sheetId="11" r:id="rId11"/>
+    <sheet name="resource skill" sheetId="12" r:id="rId12"/>
+    <sheet name="resource" sheetId="13" r:id="rId13"/>
+    <sheet name="skill" sheetId="15" r:id="rId14"/>
+    <sheet name="bucket date" sheetId="17" r:id="rId15"/>
+    <sheet name="bucket" sheetId="18" r:id="rId16"/>
+    <sheet name="parameter" sheetId="19" r:id="rId17"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="309">
   <si>
     <t>name</t>
   </si>
@@ -54,9 +55,6 @@
     <t>item</t>
   </si>
   <si>
-    <t>producing</t>
-  </si>
-  <si>
     <t>CD1-08-004</t>
   </si>
   <si>
@@ -75,9 +73,6 @@
     <t>Plasma 8mm</t>
   </si>
   <si>
-    <t>CD1-08-004 5(a)</t>
-  </si>
-  <si>
     <t>CD1-08-004 (5)a</t>
   </si>
   <si>
@@ -198,9 +193,6 @@
     <t>operation</t>
   </si>
   <si>
-    <t>buffer</t>
-  </si>
-  <si>
     <t>effective start</t>
   </si>
   <si>
@@ -949,6 +941,27 @@
   </si>
   <si>
     <t>level</t>
+  </si>
+  <si>
+    <t>CD1-08-004 @ NMI</t>
+  </si>
+  <si>
+    <t>CD1-08-004 (1)a @ NMI</t>
+  </si>
+  <si>
+    <t>CD1-08-004 (5)a @ NMI</t>
+  </si>
+  <si>
+    <t>CD1-08-004 5(b) @ NMI</t>
+  </si>
+  <si>
+    <t>CD1-08-004 5(c) @ NMI</t>
+  </si>
+  <si>
+    <t>CD1-08-004 d @ NMI</t>
+  </si>
+  <si>
+    <t>CD1-08-004 e @ NMI</t>
   </si>
 </sst>
 </file>
@@ -1291,153 +1304,104 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="20.46484375" customWidth="1"/>
-    <col min="4" max="4" width="18.53125" customWidth="1"/>
-    <col min="5" max="5" width="15.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.53125" customWidth="1"/>
+    <col min="3" max="3" width="15.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
+      <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="B4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
+      <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="B5" t="s">
         <v>14</v>
       </c>
-      <c r="E4" t="s">
+      <c r="C5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
         <v>16</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
+      <c r="B7" t="s">
         <v>18</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
+      <c r="B8" t="s">
         <v>20</v>
       </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="C8" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1446,6 +1410,37 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
@@ -1473,21 +1468,21 @@
         <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E2">
         <v>10</v>
@@ -1495,13 +1490,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3">
         <v>20</v>
@@ -1509,13 +1504,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E4">
         <v>60</v>
@@ -1523,13 +1518,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5">
         <v>15</v>
@@ -1537,13 +1532,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6">
         <v>20</v>
@@ -1551,13 +1546,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E7">
         <v>15</v>
@@ -1565,13 +1560,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D8">
         <v>10</v>
@@ -1579,13 +1574,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="B9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1593,12 +1588,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:B16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1608,27 +1603,27 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -1636,10 +1631,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -1647,10 +1642,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -1658,10 +1653,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -1669,10 +1664,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -1680,10 +1675,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -1691,10 +1686,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -1702,10 +1697,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B9" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -1713,10 +1708,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B10" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -1724,10 +1719,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B11" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -1735,10 +1730,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B12" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -1746,10 +1741,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B13" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -1757,10 +1752,10 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B14" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E14">
         <v>1</v>
@@ -1768,10 +1763,10 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B15" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -1779,10 +1774,10 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B16" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E16">
         <v>10</v>
@@ -1790,10 +1785,10 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B17" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -1801,10 +1796,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B18" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E18">
         <v>10</v>
@@ -1812,10 +1807,10 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B19" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E19">
         <v>1</v>
@@ -1823,10 +1818,10 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B20" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -1837,7 +1832,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E14"/>
   <sheetViews>
@@ -1861,32 +1856,32 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D1" t="s">
         <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B3" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3">
         <v>85</v>
@@ -1894,16 +1889,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B4" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E4">
         <v>65</v>
@@ -1911,16 +1906,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B5" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E5">
         <v>150</v>
@@ -1928,16 +1923,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B6" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E6">
         <v>45</v>
@@ -1945,16 +1940,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B7" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E7">
         <v>65</v>
@@ -1962,13 +1957,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C8">
         <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E8">
         <v>250</v>
@@ -1976,68 +1971,68 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C9">
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C11">
         <v>50</v>
       </c>
       <c r="D11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -2045,12 +2040,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1048576"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2062,37 +2057,37 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -2100,7 +2095,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D105"/>
   <sheetViews>
@@ -2115,1472 +2110,1472 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" t="s">
         <v>81</v>
-      </c>
-      <c r="B2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D2" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" t="s">
         <v>88</v>
-      </c>
-      <c r="B4" t="s">
-        <v>89</v>
-      </c>
-      <c r="C4" t="s">
-        <v>90</v>
-      </c>
-      <c r="D4" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D5" t="s">
         <v>92</v>
-      </c>
-      <c r="B5" t="s">
-        <v>93</v>
-      </c>
-      <c r="C5" t="s">
-        <v>94</v>
-      </c>
-      <c r="D5" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D6" t="s">
         <v>96</v>
-      </c>
-      <c r="B6" t="s">
-        <v>97</v>
-      </c>
-      <c r="C6" t="s">
-        <v>98</v>
-      </c>
-      <c r="D6" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C7" t="s">
         <v>96</v>
       </c>
-      <c r="B7" t="s">
-        <v>100</v>
-      </c>
-      <c r="C7" t="s">
-        <v>99</v>
-      </c>
       <c r="D7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B8" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C8" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D8" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B9" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C9" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D9" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B10" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C10" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D10" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
+        <v>89</v>
+      </c>
+      <c r="B11" t="s">
+        <v>104</v>
+      </c>
+      <c r="C11" t="s">
         <v>92</v>
       </c>
-      <c r="B11" t="s">
-        <v>107</v>
-      </c>
-      <c r="C11" t="s">
-        <v>95</v>
-      </c>
       <c r="D11" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B12" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C12" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D12" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B13" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C13" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D13" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B14" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C14" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D14" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B15" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C15" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D15" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B16" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C16" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D16" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B17" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C17" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D17" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B18" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C18" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D18" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B19" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C19" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D19" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B20" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C20" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D20" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B21" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C21" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D21" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B22" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C22" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D22" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B23" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C23" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D23" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B24" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C24" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D24" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B25" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C25" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D25" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B26" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C26" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D26" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B27" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C27" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D27" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B28" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C28" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D28" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B29" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C29" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D29" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B30" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C30" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D30" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B31" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C31" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D31" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B32" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C32" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D32" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B33" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C33" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D33" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
+        <v>85</v>
+      </c>
+      <c r="B34" t="s">
+        <v>147</v>
+      </c>
+      <c r="C34" t="s">
         <v>88</v>
       </c>
-      <c r="B34" t="s">
-        <v>150</v>
-      </c>
-      <c r="C34" t="s">
-        <v>91</v>
-      </c>
       <c r="D34" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B35" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C35" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D35" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B36" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C36" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D36" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B37" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C37" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D37" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B38" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C38" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D38" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B39" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C39" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D39" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B40" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C40" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D40" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B41" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C41" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D41" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B42" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C42" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D42" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B43" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C43" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D43" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B44" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C44" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D44" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B45" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C45" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D45" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B46" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C46" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D46" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B47" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C47" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D47" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B48" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C48" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D48" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B49" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C49" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D49" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B50" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C50" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D50" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B51" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C51" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D51" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B52" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C52" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D52" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B53" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C53" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D53" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B54" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C54" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D54" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B55" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C55" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D55" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B56" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C56" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D56" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B57" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C57" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D57" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B58" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C58" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D58" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B59" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C59" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D59" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B60" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C60" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D60" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B61" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C61" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D61" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B62" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C62" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D62" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B63" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C63" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D63" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B64" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C64" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D64" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B65" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C65" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D65" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B66" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C66" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D66" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B67" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C67" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D67" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B68" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C68" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D68" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B69" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C69" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D69" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B70" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C70" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D70" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B71" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C71" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D71" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B72" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C72" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D72" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B73" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C73" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D73" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B74" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D74" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B75" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C75" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="D75" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B76" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C76" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D76" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B77" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C77" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="D77" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B78" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C78" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D78" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B79" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C79" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D79" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B80" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C80" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="D80" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B81" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C81" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="D81" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B82" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C82" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D82" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B83" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C83" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="D83" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B84" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C84" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D84" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B85" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C85" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="D85" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B86" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C86" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D86" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B87" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C87" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D87" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B88" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C88" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="D88" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B89" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C89" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="D89" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B90" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C90" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="D90" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B91" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C91" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="D91" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B92" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C92" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D92" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B93" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C93" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D93" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B94" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C94" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="D94" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B95" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C95" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="D95" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B96" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C96" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="D96" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B97" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C97" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="D97" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B98" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C98" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D98" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B99" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C99" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D99" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B100" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C100" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D100" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B101" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C101" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="D101" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A102" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B102" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C102" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="D102" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A103" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B103" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C103" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="D103" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A104" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B104" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C104" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="D104" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A105" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B105" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C105" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="D105" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
   </sheetData>
@@ -3588,7 +3583,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -3609,15 +3604,15 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B2" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C2">
         <v>5</v>
@@ -3625,10 +3620,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B3" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="C3">
         <v>3</v>
@@ -3636,10 +3631,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B4" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -3647,10 +3642,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B5" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -3658,10 +3653,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -3672,7 +3667,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -3692,7 +3687,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -3700,35 +3695,35 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B2" s="1">
         <v>42005.5</v>
       </c>
       <c r="C2" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B3" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C3" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B4" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C4" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
   </sheetData>
@@ -3738,9 +3733,141 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="20.46484375" customWidth="1"/>
+    <col min="4" max="4" width="18.53125" customWidth="1"/>
+    <col min="5" max="5" width="15.796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>303</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>304</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>305</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>306</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>307</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>308</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
@@ -3753,57 +3880,57 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
         <v>24</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>25</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>26</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>27</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>28</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>29</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>30</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>31</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>32</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>33</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>34</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>35</v>
-      </c>
-      <c r="M1" t="s">
-        <v>36</v>
-      </c>
-      <c r="N1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -3833,10 +3960,10 @@
         <v>0</v>
       </c>
       <c r="M2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="N2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -3844,7 +3971,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -3862,12 +3989,12 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -3878,7 +4005,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -3895,7 +4022,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
   </sheetData>
@@ -3903,11 +4030,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -3923,7 +4050,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C1" t="s">
         <v>4</v>
@@ -3932,45 +4059,45 @@
         <v>5</v>
       </c>
       <c r="E1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" t="s">
         <v>45</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>46</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" t="s">
         <v>47</v>
-      </c>
-      <c r="H1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" t="s">
+        <v>294</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" t="s">
         <v>50</v>
       </c>
-      <c r="B2" t="s">
-        <v>297</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F2" t="s">
-        <v>52</v>
-      </c>
       <c r="G2" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="H2">
         <v>200</v>
@@ -3984,25 +4111,25 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B3" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G3" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="H3">
         <v>200</v>
@@ -4016,25 +4143,25 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="B4" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G4" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="H4">
         <v>200</v>
@@ -4048,25 +4175,25 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="B5" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G5" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="H5">
         <v>200</v>
@@ -4083,12 +4210,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:D9"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4099,13 +4226,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B1" t="s">
-        <v>54</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -4113,198 +4240,198 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5">
         <v>-1</v>
       </c>
       <c r="D5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C7">
         <v>-1</v>
       </c>
       <c r="D7" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C9">
         <v>-2</v>
       </c>
       <c r="D9" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10">
         <v>-1</v>
       </c>
       <c r="D10" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C12">
         <v>-1</v>
       </c>
       <c r="D12" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C14">
         <v>-1</v>
       </c>
       <c r="D14" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="B15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C15">
         <v>-1</v>
       </c>
       <c r="D15" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -4312,7 +4439,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
@@ -4331,45 +4458,45 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -4377,11 +4504,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
@@ -4393,27 +4520,27 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E1" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -4421,27 +4548,27 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -4449,27 +4576,27 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -4477,27 +4604,27 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -4505,27 +4632,27 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -4533,27 +4660,27 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C11" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -4561,27 +4688,27 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C13" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -4589,50 +4716,19 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C15" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>303</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>41</v>
+        <v>300</v>
       </c>
     </row>
   </sheetData>

</xml_diff>